<commit_message>
[DOC] - analyse algo de recherche fini
</commit_message>
<xml_diff>
--- a/ComparaisonJeu.xlsx
+++ b/ComparaisonJeu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell G3\Desktop\Devoirs\BUT3\ia\SAE-IA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\IUT\3A\S5\IntroductionIA\SAE-IA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B44F619-1A58-4043-9AA5-6200D908442C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B32079D-BE48-4138-978C-64D470BDB63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5F2CFC5-267E-43DF-97D2-5A5BEB9D2875}"/>
+    <workbookView xWindow="14190" yWindow="0" windowWidth="14610" windowHeight="15480" xr2:uid="{F5F2CFC5-267E-43DF-97D2-5A5BEB9D2875}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="112">
   <si>
     <t>taille jeu</t>
   </si>
@@ -141,16 +141,253 @@
   </si>
   <si>
     <t>Tableur en dessous juste pour les graphiques</t>
+  </si>
+  <si>
+    <t>Algo</t>
+  </si>
+  <si>
+    <t>Problème</t>
+  </si>
+  <si>
+    <t>rnd</t>
+  </si>
+  <si>
+    <t>bfs</t>
+  </si>
+  <si>
+    <t>dfs</t>
+  </si>
+  <si>
+    <t>ucs</t>
+  </si>
+  <si>
+    <t>gfs</t>
+  </si>
+  <si>
+    <t>astar</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>Coût</t>
+  </si>
+  <si>
+    <t>états explorés</t>
+  </si>
+  <si>
+    <t>Temps</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Problème (dummy)</t>
+  </si>
+  <si>
+    <t>1572.4948775695832</t>
+  </si>
+  <si>
+    <t>0,007 sec</t>
+  </si>
+  <si>
+    <t>0,004 sec</t>
+  </si>
+  <si>
+    <t>1719.4506178846962</t>
+  </si>
+  <si>
+    <t>0,011 sec</t>
+  </si>
+  <si>
+    <t>30980.752615841193</t>
+  </si>
+  <si>
+    <t>0,013 sec</t>
+  </si>
+  <si>
+    <t>0,009 sec</t>
+  </si>
+  <si>
+    <t>2282.165489708158</t>
+  </si>
+  <si>
+    <t>n~10^2 k = 5</t>
+  </si>
+  <si>
+    <t>Très facile</t>
+  </si>
+  <si>
+    <t>Très simple</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Moyen</t>
+  </si>
+  <si>
+    <t>Difficile</t>
+  </si>
+  <si>
+    <t>Très difficile</t>
+  </si>
+  <si>
+    <t>Taille(n)</t>
+  </si>
+  <si>
+    <t>Facteur de branchement (k)</t>
+  </si>
+  <si>
+    <t>Graine</t>
+  </si>
+  <si>
+    <t>Difficulté</t>
+  </si>
+  <si>
+    <t>n~10^2 k = 2</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>0,008 sec</t>
+  </si>
+  <si>
+    <t>facile</t>
+  </si>
+  <si>
+    <t>n~10^3 k = 3</t>
+  </si>
+  <si>
+    <t>n~10^4 k = 4</t>
+  </si>
+  <si>
+    <t>8,049 sec</t>
+  </si>
+  <si>
+    <t>7521.319105999773</t>
+  </si>
+  <si>
+    <t>3,949 sec</t>
+  </si>
+  <si>
+    <t>3971.0530517419766</t>
+  </si>
+  <si>
+    <t>8,304 sec</t>
+  </si>
+  <si>
+    <t>4119235.131724489</t>
+  </si>
+  <si>
+    <t>10,751 sec</t>
+  </si>
+  <si>
+    <t>3526.4692773849947</t>
+  </si>
+  <si>
+    <t>18,005 sec</t>
+  </si>
+  <si>
+    <t>16220.209153486552</t>
+  </si>
+  <si>
+    <t>8,226 sec</t>
+  </si>
+  <si>
+    <t>n~50 000 k = 5</t>
+  </si>
+  <si>
+    <t>4069.479721959591</t>
+  </si>
+  <si>
+    <t>1.8444604239156943E7</t>
+  </si>
+  <si>
+    <t>522,136 sec</t>
+  </si>
+  <si>
+    <t>645,514 sec</t>
+  </si>
+  <si>
+    <t>3592.979834481036</t>
+  </si>
+  <si>
+    <t>1013,307 sec</t>
+  </si>
+  <si>
+    <t>16723.790765091595</t>
+  </si>
+  <si>
+    <t>383,563 sec</t>
+  </si>
+  <si>
+    <t>956,672 sec</t>
+  </si>
+  <si>
+    <t>7652.954675242736</t>
+  </si>
+  <si>
+    <t>4646.435242513757</t>
+  </si>
+  <si>
+    <t>38943.89746267833</t>
+  </si>
+  <si>
+    <t>7049.501460528446</t>
+  </si>
+  <si>
+    <t>0,01 sec</t>
+  </si>
+  <si>
+    <t>fait</t>
+  </si>
+  <si>
+    <t>2548.9715885223704</t>
+  </si>
+  <si>
+    <t>0,028 sec</t>
+  </si>
+  <si>
+    <t>0,051 sec</t>
+  </si>
+  <si>
+    <t>12504.048140861101</t>
+  </si>
+  <si>
+    <t>0,032 sec</t>
+  </si>
+  <si>
+    <t>147287.14433960532</t>
+  </si>
+  <si>
+    <t>0,025 sec</t>
+  </si>
+  <si>
+    <t>0,036 sec</t>
+  </si>
+  <si>
+    <t>7640.800462439074</t>
+  </si>
+  <si>
+    <t>0,044 sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -244,11 +481,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -275,6 +583,49 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -295,7 +646,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -745,7 +1096,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2352,11 +2703,55 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>173812</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>62112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>597259</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>5308</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2781264-3F01-92EC-D6F3-FA5DD58EFD5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9400267" y="13766739"/>
+          <a:ext cx="5797253" cy="327039"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2672,25 +3067,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BEEA06-2717-4799-B2CC-E672E72977A1}">
-  <dimension ref="A3:G35"/>
+  <dimension ref="A3:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="90" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2713,7 +3108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -2736,7 +3131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="8">
         <v>17596</v>
       </c>
@@ -2747,7 +3142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -2770,7 +3165,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="8">
         <v>64925</v>
       </c>
@@ -2781,7 +3176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2804,7 +3199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="8">
         <v>27065</v>
       </c>
@@ -2815,7 +3210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -2838,7 +3233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="8">
         <v>35386</v>
       </c>
@@ -2849,7 +3244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2872,7 +3267,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" s="8">
         <v>251192</v>
       </c>
@@ -2883,14 +3278,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>31</v>
       </c>
@@ -2901,7 +3296,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
@@ -2915,7 +3310,7 @@
         <v>17596</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -2929,7 +3324,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" s="7" t="s">
         <v>24</v>
       </c>
@@ -2940,7 +3335,7 @@
         <v>64925</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
@@ -2951,7 +3346,7 @@
         <v>27065</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C22" s="7" t="s">
         <v>28</v>
       </c>
@@ -2962,7 +3357,7 @@
         <v>35386</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>21</v>
       </c>
@@ -2973,7 +3368,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
         <v>25</v>
       </c>
@@ -2984,7 +3379,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
         <v>27</v>
       </c>
@@ -2995,7 +3390,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" s="7" t="s">
         <v>17</v>
       </c>
@@ -3006,7 +3401,7 @@
         <v>251192</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="6" t="s">
         <v>18</v>
       </c>
@@ -3017,8 +3412,8 @@
         <v>550000</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
         <v>14</v>
       </c>
@@ -3029,7 +3424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
         <v>6</v>
       </c>
@@ -3040,7 +3435,7 @@
         <v>17596</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="4" t="s">
         <v>32</v>
       </c>
@@ -3051,7 +3446,7 @@
         <v>64925</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
         <v>10</v>
       </c>
@@ -3062,7 +3457,7 @@
         <v>27065</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C34" s="4" t="s">
         <v>33</v>
       </c>
@@ -3073,7 +3468,7 @@
         <v>35386</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
         <v>15</v>
       </c>
@@ -3084,8 +3479,988 @@
         <v>251192</v>
       </c>
     </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="4">
+        <v>450</v>
+      </c>
+      <c r="E45" s="4">
+        <v>7</v>
+      </c>
+      <c r="F45" s="12">
+        <v>31</v>
+      </c>
+      <c r="G45" s="13">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="4">
+        <v>450</v>
+      </c>
+      <c r="E46" s="4">
+        <v>3</v>
+      </c>
+      <c r="F46" s="12">
+        <v>21</v>
+      </c>
+      <c r="G46" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="4">
+        <v>575</v>
+      </c>
+      <c r="E47" s="4">
+        <v>11</v>
+      </c>
+      <c r="F47" s="12">
+        <v>29</v>
+      </c>
+      <c r="G47" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="4">
+        <v>418</v>
+      </c>
+      <c r="E48" s="4">
+        <v>5</v>
+      </c>
+      <c r="F48" s="12">
+        <v>31</v>
+      </c>
+      <c r="G48" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="4">
+        <v>450</v>
+      </c>
+      <c r="E49" s="4">
+        <v>3</v>
+      </c>
+      <c r="F49" s="12">
+        <v>10</v>
+      </c>
+      <c r="G49" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="4">
+        <v>418</v>
+      </c>
+      <c r="E50" s="4">
+        <v>4</v>
+      </c>
+      <c r="F50" s="12">
+        <v>16</v>
+      </c>
+      <c r="G50" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E56" s="4">
+        <v>9</v>
+      </c>
+      <c r="F56" s="12">
+        <v>472</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="4">
+        <v>5</v>
+      </c>
+      <c r="F57" s="12">
+        <v>497</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E58" s="4">
+        <v>62</v>
+      </c>
+      <c r="F58" s="12">
+        <v>312</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" s="4">
+        <v>9</v>
+      </c>
+      <c r="F59" s="12">
+        <v>537</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" s="4">
+        <v>4</v>
+      </c>
+      <c r="F60" s="12">
+        <v>32</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" s="4">
+        <v>6</v>
+      </c>
+      <c r="F61" s="12">
+        <v>147</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C66" s="4">
+        <v>100</v>
+      </c>
+      <c r="D66" s="4">
+        <v>2</v>
+      </c>
+      <c r="E66" s="16">
+        <v>786597272</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D67" s="4">
+        <v>3</v>
+      </c>
+      <c r="E67" s="17">
+        <v>1142418294</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D68" s="4">
+        <v>4</v>
+      </c>
+      <c r="E68" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" s="4">
+        <v>50000</v>
+      </c>
+      <c r="D69" s="4">
+        <v>5</v>
+      </c>
+      <c r="E69" s="17">
+        <v>1322200015</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" s="15">
+        <v>100000</v>
+      </c>
+      <c r="D70" s="15">
+        <v>6</v>
+      </c>
+      <c r="E70" s="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E75" s="4">
+        <v>14</v>
+      </c>
+      <c r="F75" s="12">
+        <v>200</v>
+      </c>
+      <c r="G75" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E76" s="4">
+        <v>9</v>
+      </c>
+      <c r="F76" s="12">
+        <v>190</v>
+      </c>
+      <c r="G76" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E77" s="4">
+        <v>76</v>
+      </c>
+      <c r="F77" s="12">
+        <v>170</v>
+      </c>
+      <c r="G77" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E78" s="4">
+        <v>11</v>
+      </c>
+      <c r="F78" s="12">
+        <v>208</v>
+      </c>
+      <c r="G78" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E79" s="4">
+        <v>17</v>
+      </c>
+      <c r="F79" s="12">
+        <v>226</v>
+      </c>
+      <c r="G79" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E80" s="15">
+        <v>11</v>
+      </c>
+      <c r="F80" s="22">
+        <v>210</v>
+      </c>
+      <c r="G80" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E85" s="4">
+        <v>17</v>
+      </c>
+      <c r="F85" s="12">
+        <v>1787</v>
+      </c>
+      <c r="G85" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E86" s="4">
+        <v>7</v>
+      </c>
+      <c r="F86" s="12">
+        <v>1562</v>
+      </c>
+      <c r="G86" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E87" s="4">
+        <v>285</v>
+      </c>
+      <c r="F87" s="12">
+        <v>857</v>
+      </c>
+      <c r="G87" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E88" s="4">
+        <v>10</v>
+      </c>
+      <c r="F88" s="12">
+        <v>1247</v>
+      </c>
+      <c r="G88" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E89" s="4">
+        <v>42</v>
+      </c>
+      <c r="F89" s="12">
+        <v>3302</v>
+      </c>
+      <c r="G89" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E90" s="15">
+        <v>9</v>
+      </c>
+      <c r="F90" s="22">
+        <v>533</v>
+      </c>
+      <c r="G90" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E95" s="4">
+        <v>20</v>
+      </c>
+      <c r="F95" s="12">
+        <v>35394</v>
+      </c>
+      <c r="G95" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E96" s="4">
+        <v>8</v>
+      </c>
+      <c r="F96" s="12">
+        <v>23150</v>
+      </c>
+      <c r="G96" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E97" s="4">
+        <v>7693</v>
+      </c>
+      <c r="F97" s="12">
+        <v>32918</v>
+      </c>
+      <c r="G97" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E98" s="4">
+        <v>15</v>
+      </c>
+      <c r="F98" s="12">
+        <v>49703</v>
+      </c>
+      <c r="G98" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E99" s="4">
+        <v>96</v>
+      </c>
+      <c r="F99" s="12">
+        <v>109890</v>
+      </c>
+      <c r="G99" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E100" s="15">
+        <v>16</v>
+      </c>
+      <c r="F100" s="22">
+        <v>32862</v>
+      </c>
+      <c r="G100" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G105" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E106" s="4">
+        <v>8</v>
+      </c>
+      <c r="F106" s="12">
+        <v>192572</v>
+      </c>
+      <c r="G106" s="24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E107" s="4">
+        <v>34374</v>
+      </c>
+      <c r="F107" s="12">
+        <v>174242</v>
+      </c>
+      <c r="G107" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E108" s="4">
+        <v>19</v>
+      </c>
+      <c r="F108" s="12">
+        <v>322913</v>
+      </c>
+      <c r="G108" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E109" s="4">
+        <v>143</v>
+      </c>
+      <c r="F109" s="12">
+        <v>113072</v>
+      </c>
+      <c r="G109" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D110" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E110" s="15">
+        <v>18</v>
+      </c>
+      <c r="F110" s="22">
+        <v>199317</v>
+      </c>
+      <c r="G110" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>